<commit_message>
add toolbox and alice/jennifer's scripts for reference
</commit_message>
<xml_diff>
--- a/emhmm-toolbox/demo_cocluster/brm-data/stimuli-info.xlsx
+++ b/emhmm-toolbox/demo_cocluster/brm-data/stimuli-info.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shaderein/Work/XAI/emhmm-toolbox/demo_cocluster/brm-data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249AEDA5-7F43-254A-90DA-C7A504D7474C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28380" yWindow="10515" windowWidth="19440" windowHeight="15000"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -399,7 +405,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -737,23 +743,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C121"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -770,7 +776,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -781,13 +787,13 @@
         <v>639</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E2">
         <v>479</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -798,13 +804,13 @@
         <v>639</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E3">
         <v>479</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -815,13 +821,13 @@
         <v>639</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E4">
         <v>479</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -832,13 +838,13 @@
         <v>639</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E5">
         <v>479</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -849,13 +855,13 @@
         <v>639</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E6">
         <v>479</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -866,13 +872,13 @@
         <v>639</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E7">
         <v>479</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -883,13 +889,13 @@
         <v>639</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E8">
         <v>479</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -900,13 +906,13 @@
         <v>639</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E9">
         <v>479</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -917,13 +923,13 @@
         <v>639</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E10">
         <v>479</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -934,13 +940,13 @@
         <v>639</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E11">
         <v>479</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -951,13 +957,13 @@
         <v>639</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E12">
         <v>479</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -968,13 +974,13 @@
         <v>639</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E13">
         <v>479</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -985,13 +991,13 @@
         <v>639</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E14">
         <v>479</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1002,13 +1008,13 @@
         <v>639</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E15">
         <v>479</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1019,13 +1025,13 @@
         <v>639</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E16">
         <v>479</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1036,13 +1042,13 @@
         <v>639</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E17">
         <v>479</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1053,13 +1059,13 @@
         <v>639</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E18">
         <v>479</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1070,13 +1076,13 @@
         <v>639</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E19">
         <v>479</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1087,13 +1093,13 @@
         <v>639</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E20">
         <v>479</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1104,13 +1110,13 @@
         <v>639</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E21">
         <v>479</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1121,13 +1127,13 @@
         <v>639</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E22">
         <v>479</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1138,13 +1144,13 @@
         <v>639</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E23">
         <v>479</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1155,13 +1161,13 @@
         <v>639</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E24">
         <v>479</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1172,13 +1178,13 @@
         <v>639</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E25">
         <v>479</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1189,13 +1195,13 @@
         <v>639</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E26">
         <v>479</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -1206,13 +1212,13 @@
         <v>639</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E27">
         <v>479</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -1223,13 +1229,13 @@
         <v>639</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E28">
         <v>479</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>32</v>
       </c>
@@ -1240,13 +1246,13 @@
         <v>639</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E29">
         <v>479</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1257,13 +1263,13 @@
         <v>639</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E30">
         <v>479</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -1274,13 +1280,13 @@
         <v>639</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E31">
         <v>479</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>35</v>
       </c>
@@ -1291,13 +1297,13 @@
         <v>639</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E32">
         <v>479</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -1308,13 +1314,13 @@
         <v>639</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E33">
         <v>479</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -1325,13 +1331,13 @@
         <v>639</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E34">
         <v>479</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -1342,13 +1348,13 @@
         <v>639</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E35">
         <v>479</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1359,13 +1365,13 @@
         <v>639</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E36">
         <v>479</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>40</v>
       </c>
@@ -1376,13 +1382,13 @@
         <v>639</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E37">
         <v>479</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -1393,13 +1399,13 @@
         <v>639</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E38">
         <v>479</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -1410,13 +1416,13 @@
         <v>639</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E39">
         <v>479</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -1427,13 +1433,13 @@
         <v>639</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E40">
         <v>479</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -1444,13 +1450,13 @@
         <v>639</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E41">
         <v>479</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>45</v>
       </c>
@@ -1461,13 +1467,13 @@
         <v>639</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E42">
         <v>479</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>46</v>
       </c>
@@ -1478,13 +1484,13 @@
         <v>639</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E43">
         <v>479</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -1495,13 +1501,13 @@
         <v>639</v>
       </c>
       <c r="D44">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E44">
         <v>479</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>48</v>
       </c>
@@ -1512,13 +1518,13 @@
         <v>639</v>
       </c>
       <c r="D45">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E45">
         <v>479</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -1529,13 +1535,13 @@
         <v>639</v>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E46">
         <v>479</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -1546,13 +1552,13 @@
         <v>639</v>
       </c>
       <c r="D47">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E47">
         <v>479</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -1563,13 +1569,13 @@
         <v>639</v>
       </c>
       <c r="D48">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E48">
         <v>479</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>52</v>
       </c>
@@ -1580,13 +1586,13 @@
         <v>639</v>
       </c>
       <c r="D49">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E49">
         <v>479</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>53</v>
       </c>
@@ -1597,13 +1603,13 @@
         <v>639</v>
       </c>
       <c r="D50">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E50">
         <v>479</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>54</v>
       </c>
@@ -1614,13 +1620,13 @@
         <v>639</v>
       </c>
       <c r="D51">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E51">
         <v>479</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>55</v>
       </c>
@@ -1631,13 +1637,13 @@
         <v>639</v>
       </c>
       <c r="D52">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E52">
         <v>479</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>56</v>
       </c>
@@ -1648,13 +1654,13 @@
         <v>639</v>
       </c>
       <c r="D53">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E53">
         <v>479</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>57</v>
       </c>
@@ -1665,13 +1671,13 @@
         <v>639</v>
       </c>
       <c r="D54">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E54">
         <v>479</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>58</v>
       </c>
@@ -1682,13 +1688,13 @@
         <v>639</v>
       </c>
       <c r="D55">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E55">
         <v>479</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>59</v>
       </c>
@@ -1699,13 +1705,13 @@
         <v>639</v>
       </c>
       <c r="D56">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E56">
         <v>479</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>60</v>
       </c>
@@ -1716,13 +1722,13 @@
         <v>639</v>
       </c>
       <c r="D57">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E57">
         <v>479</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>61</v>
       </c>
@@ -1733,13 +1739,13 @@
         <v>639</v>
       </c>
       <c r="D58">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E58">
         <v>479</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>62</v>
       </c>
@@ -1750,13 +1756,13 @@
         <v>639</v>
       </c>
       <c r="D59">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E59">
         <v>479</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>63</v>
       </c>
@@ -1767,13 +1773,13 @@
         <v>639</v>
       </c>
       <c r="D60">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E60">
         <v>479</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>64</v>
       </c>
@@ -1784,13 +1790,13 @@
         <v>639</v>
       </c>
       <c r="D61">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E61">
         <v>479</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>65</v>
       </c>
@@ -1801,13 +1807,13 @@
         <v>639</v>
       </c>
       <c r="D62">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E62">
         <v>479</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>66</v>
       </c>
@@ -1818,13 +1824,13 @@
         <v>639</v>
       </c>
       <c r="D63">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E63">
         <v>479</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>67</v>
       </c>
@@ -1835,13 +1841,13 @@
         <v>639</v>
       </c>
       <c r="D64">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E64">
         <v>479</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>68</v>
       </c>
@@ -1852,13 +1858,13 @@
         <v>639</v>
       </c>
       <c r="D65">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E65">
         <v>479</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>69</v>
       </c>
@@ -1869,13 +1875,13 @@
         <v>639</v>
       </c>
       <c r="D66">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E66">
         <v>479</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>70</v>
       </c>
@@ -1886,13 +1892,13 @@
         <v>639</v>
       </c>
       <c r="D67">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E67">
         <v>479</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>71</v>
       </c>
@@ -1903,13 +1909,13 @@
         <v>639</v>
       </c>
       <c r="D68">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E68">
         <v>479</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>72</v>
       </c>
@@ -1920,13 +1926,13 @@
         <v>639</v>
       </c>
       <c r="D69">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E69">
         <v>479</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>73</v>
       </c>
@@ -1937,13 +1943,13 @@
         <v>639</v>
       </c>
       <c r="D70">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E70">
         <v>479</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>74</v>
       </c>
@@ -1954,13 +1960,13 @@
         <v>639</v>
       </c>
       <c r="D71">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E71">
         <v>479</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>75</v>
       </c>
@@ -1971,13 +1977,13 @@
         <v>639</v>
       </c>
       <c r="D72">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E72">
         <v>479</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>76</v>
       </c>
@@ -1988,13 +1994,13 @@
         <v>639</v>
       </c>
       <c r="D73">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E73">
         <v>479</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>77</v>
       </c>
@@ -2005,13 +2011,13 @@
         <v>639</v>
       </c>
       <c r="D74">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E74">
         <v>479</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>78</v>
       </c>
@@ -2022,13 +2028,13 @@
         <v>639</v>
       </c>
       <c r="D75">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E75">
         <v>479</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>79</v>
       </c>
@@ -2039,13 +2045,13 @@
         <v>639</v>
       </c>
       <c r="D76">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E76">
         <v>479</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>80</v>
       </c>
@@ -2056,13 +2062,13 @@
         <v>639</v>
       </c>
       <c r="D77">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E77">
         <v>479</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>81</v>
       </c>
@@ -2073,13 +2079,13 @@
         <v>639</v>
       </c>
       <c r="D78">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E78">
         <v>479</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>82</v>
       </c>
@@ -2090,13 +2096,13 @@
         <v>639</v>
       </c>
       <c r="D79">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E79">
         <v>479</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>83</v>
       </c>
@@ -2107,13 +2113,13 @@
         <v>639</v>
       </c>
       <c r="D80">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E80">
         <v>479</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>84</v>
       </c>
@@ -2124,13 +2130,13 @@
         <v>639</v>
       </c>
       <c r="D81">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E81">
         <v>479</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>85</v>
       </c>
@@ -2141,13 +2147,13 @@
         <v>639</v>
       </c>
       <c r="D82">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E82">
         <v>479</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>86</v>
       </c>
@@ -2158,13 +2164,13 @@
         <v>639</v>
       </c>
       <c r="D83">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E83">
         <v>479</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>87</v>
       </c>
@@ -2175,13 +2181,13 @@
         <v>639</v>
       </c>
       <c r="D84">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E84">
         <v>479</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>88</v>
       </c>
@@ -2192,13 +2198,13 @@
         <v>639</v>
       </c>
       <c r="D85">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E85">
         <v>479</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>89</v>
       </c>
@@ -2209,13 +2215,13 @@
         <v>639</v>
       </c>
       <c r="D86">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E86">
         <v>479</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>90</v>
       </c>
@@ -2226,13 +2232,13 @@
         <v>639</v>
       </c>
       <c r="D87">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E87">
         <v>479</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>91</v>
       </c>
@@ -2243,13 +2249,13 @@
         <v>639</v>
       </c>
       <c r="D88">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E88">
         <v>479</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>92</v>
       </c>
@@ -2260,13 +2266,13 @@
         <v>639</v>
       </c>
       <c r="D89">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E89">
         <v>479</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>93</v>
       </c>
@@ -2277,13 +2283,13 @@
         <v>639</v>
       </c>
       <c r="D90">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E90">
         <v>479</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>94</v>
       </c>
@@ -2294,13 +2300,13 @@
         <v>639</v>
       </c>
       <c r="D91">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E91">
         <v>479</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>95</v>
       </c>
@@ -2311,13 +2317,13 @@
         <v>639</v>
       </c>
       <c r="D92">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E92">
         <v>479</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>96</v>
       </c>
@@ -2328,13 +2334,13 @@
         <v>639</v>
       </c>
       <c r="D93">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E93">
         <v>479</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>97</v>
       </c>
@@ -2345,13 +2351,13 @@
         <v>639</v>
       </c>
       <c r="D94">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E94">
         <v>479</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>98</v>
       </c>
@@ -2362,13 +2368,13 @@
         <v>639</v>
       </c>
       <c r="D95">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E95">
         <v>479</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>99</v>
       </c>
@@ -2379,13 +2385,13 @@
         <v>639</v>
       </c>
       <c r="D96">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E96">
         <v>479</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>100</v>
       </c>
@@ -2396,13 +2402,13 @@
         <v>639</v>
       </c>
       <c r="D97">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E97">
         <v>479</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>101</v>
       </c>
@@ -2413,13 +2419,13 @@
         <v>639</v>
       </c>
       <c r="D98">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E98">
         <v>479</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>102</v>
       </c>
@@ -2430,13 +2436,13 @@
         <v>639</v>
       </c>
       <c r="D99">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E99">
         <v>479</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>103</v>
       </c>
@@ -2447,13 +2453,13 @@
         <v>639</v>
       </c>
       <c r="D100">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E100">
         <v>479</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>104</v>
       </c>
@@ -2464,13 +2470,13 @@
         <v>639</v>
       </c>
       <c r="D101">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E101">
         <v>479</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>105</v>
       </c>
@@ -2481,13 +2487,13 @@
         <v>639</v>
       </c>
       <c r="D102">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E102">
         <v>479</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>106</v>
       </c>
@@ -2498,13 +2504,13 @@
         <v>639</v>
       </c>
       <c r="D103">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E103">
         <v>479</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>107</v>
       </c>
@@ -2515,13 +2521,13 @@
         <v>639</v>
       </c>
       <c r="D104">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E104">
         <v>479</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>108</v>
       </c>
@@ -2532,13 +2538,13 @@
         <v>639</v>
       </c>
       <c r="D105">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E105">
         <v>479</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>109</v>
       </c>
@@ -2549,13 +2555,13 @@
         <v>639</v>
       </c>
       <c r="D106">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E106">
         <v>479</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>110</v>
       </c>
@@ -2566,13 +2572,13 @@
         <v>639</v>
       </c>
       <c r="D107">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E107">
         <v>479</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>111</v>
       </c>
@@ -2583,13 +2589,13 @@
         <v>639</v>
       </c>
       <c r="D108">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E108">
         <v>479</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>112</v>
       </c>
@@ -2600,13 +2606,13 @@
         <v>639</v>
       </c>
       <c r="D109">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E109">
         <v>479</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>113</v>
       </c>
@@ -2617,13 +2623,13 @@
         <v>639</v>
       </c>
       <c r="D110">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E110">
         <v>479</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>114</v>
       </c>
@@ -2634,13 +2640,13 @@
         <v>639</v>
       </c>
       <c r="D111">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E111">
         <v>479</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>115</v>
       </c>
@@ -2651,13 +2657,13 @@
         <v>639</v>
       </c>
       <c r="D112">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E112">
         <v>479</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>116</v>
       </c>
@@ -2668,13 +2674,13 @@
         <v>639</v>
       </c>
       <c r="D113">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E113">
         <v>479</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>117</v>
       </c>
@@ -2685,13 +2691,13 @@
         <v>639</v>
       </c>
       <c r="D114">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E114">
         <v>479</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>118</v>
       </c>
@@ -2702,13 +2708,13 @@
         <v>639</v>
       </c>
       <c r="D115">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E115">
         <v>479</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>119</v>
       </c>
@@ -2719,13 +2725,13 @@
         <v>639</v>
       </c>
       <c r="D116">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E116">
         <v>479</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>120</v>
       </c>
@@ -2736,13 +2742,13 @@
         <v>639</v>
       </c>
       <c r="D117">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E117">
         <v>479</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>121</v>
       </c>
@@ -2753,13 +2759,13 @@
         <v>639</v>
       </c>
       <c r="D118">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E118">
         <v>479</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>122</v>
       </c>
@@ -2770,13 +2776,13 @@
         <v>639</v>
       </c>
       <c r="D119">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E119">
         <v>479</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>123</v>
       </c>
@@ -2787,13 +2793,13 @@
         <v>639</v>
       </c>
       <c r="D120">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E120">
         <v>479</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>124</v>
       </c>
@@ -2804,7 +2810,7 @@
         <v>639</v>
       </c>
       <c r="D121">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="E121">
         <v>479</v>
@@ -2812,5 +2818,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>